<commit_message>
_ Mise à jour modèle avec planification   * Planification complete des capacités installées     - Possibilité de donner l'âge des capacités installées lors du début de la simulation   * Case study acier en France (données à consolider) de 2015 à 2050     - Jusqu'en 2030 chemin fixé par les annonces d'Arcelor Mittal     - Optimisation complete après 2030 avec pour hypothèses une augmentation du coût carbone et du prix des fossiles avec une baisse des coûts de production du biogaz et d'utilisation de biomasse
  * Extraction de données et affichage de graphiques avec Steel_planification.py

_ Mise à jour de l'Excel d'entrée parameters_planification.xlsx en conséquence
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/Resources_characteristics.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/Resources_characteristics.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76892F99-006D-DF4C-9F3A-0594AA00626F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA529B0C-D51C-4790-AD3E-E9917184138B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="22260" windowHeight="12636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,16 +16,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -39,24 +29,6 @@
     <t>calorific_value_MWh_t</t>
   </si>
   <si>
-    <t>hydrogen</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>biomass</t>
-  </si>
-  <si>
-    <t>gas</t>
-  </si>
-  <si>
-    <t>coal</t>
-  </si>
-  <si>
-    <t>oil</t>
-  </si>
-  <si>
     <t>https://world-nuclear.org/information-library/facts-and-figures/heat-values-of-various-fuels.aspx</t>
   </si>
   <si>
@@ -64,6 +36,24 @@
   </si>
   <si>
     <t>fuel_emissions_tCO2_MWh</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Biomass</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
   </si>
 </sst>
 </file>
@@ -385,17 +375,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,12 +393,12 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <f>0.27778*42</f>
@@ -419,7 +409,7 @@
         <v>0.32666666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -432,9 +422,9 @@
         <v>0.39192991895395379</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <f>0.27778*42</f>
@@ -445,9 +435,9 @@
         <v>0.18086378737541528</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <f>0.27778*16</f>
@@ -458,9 +448,9 @@
         <v>0.22499820001439985</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -469,9 +459,9 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <f>0.27778*120</f>
@@ -494,16 +484,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>